<commit_message>
upload log to database
</commit_message>
<xml_diff>
--- a/battlelogs.xlsx
+++ b/battlelogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyangliu/Desktop/NFSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70DC9CA7-F66F-8147-BE3C-885EDA3DC8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E336E2-B9C5-5749-A5B5-A8235F92B966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="16660" xr2:uid="{A5CEE887-67F8-5A40-842F-6AF87604A1E5}"/>
   </bookViews>
@@ -436,9 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE61074F-0FF1-934F-BDD1-F45D66845E69}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>